<commit_message>
creating theoretical vs recorded drift velocity graph
Plotting the theoretical drift velocity vs the ave. drift velocity recorded.
</commit_message>
<xml_diff>
--- a/closest_alpha_pos_1_to_101_MaxC_60000_Grad_0.000405.xlsx
+++ b/closest_alpha_pos_1_to_101_MaxC_60000_Grad_0.000405.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Moar Documents\GitHub\Run_Tumble_Gillespie_Diffusion_Equation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B25D05F-956B-4EDD-914B-810C7FB91A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0481DA-8879-44E0-B97F-3711191DEB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{67997574-F618-4EAD-A196-F9F66C722695}"/>
   </bookViews>
@@ -3424,8 +3424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F159FE-D3DB-49C1-B473-4E87221778F1}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>